<commit_message>
Wrote out "Active" in Table 5
</commit_message>
<xml_diff>
--- a/S.Table5.xlsx
+++ b/S.Table5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacea\OneDrive\Documents\GitHub\MultiomicsFrackingSupplemental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF65758C-86D8-484D-857C-E083031D9D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A9C723-CB8A-438D-B4F1-7D478F3C0F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,13 +63,13 @@
     <t>Water 16S rRNA gene HF+ samples</t>
   </si>
   <si>
-    <t>WellPad_Ac</t>
-  </si>
-  <si>
     <t>Supplemental Table 5: Well pad and active wells variation explained among HF samples only for each dataset. Paired datasets were not subject to this analysis, as their respective HF- samples were excluded.</t>
   </si>
   <si>
     <t>Metatranscriptomics microbial composition (metatranscriptome) HF+ samples</t>
+  </si>
+  <si>
+    <t>WellPad_Active</t>
   </si>
 </sst>
 </file>
@@ -399,14 +399,14 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -531,7 +531,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>8.3199809020000001E-2</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>0.28024803949999999</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>0.18958987729999999</v>
@@ -586,12 +586,12 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>4.2472593029999998E-2</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>6.743520033E-2</v>

</xml_diff>

<commit_message>
Changed HF+ to UOG+ for consistency
</commit_message>
<xml_diff>
--- a/S.Table5.xlsx
+++ b/S.Table5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacea\OneDrive\Documents\GitHub\MultiomicsFrackingSupplemental\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Jeremy\Documents\RW\May.2022\fracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A9C723-CB8A-438D-B4F1-7D478F3C0F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B831EF-BF42-4FAA-B060-26C7BB69F009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="3555" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S.Table5" sheetId="1" r:id="rId1"/>
@@ -51,25 +51,25 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Metatranscriptomics antimicrobial resistance genes HF+ samples</t>
-  </si>
-  <si>
-    <t>Metatranscriptomics HF+ samples</t>
-  </si>
-  <si>
-    <t>Sediment 16S rRNA gene HF+ samples</t>
-  </si>
-  <si>
-    <t>Water 16S rRNA gene HF+ samples</t>
-  </si>
-  <si>
-    <t>Supplemental Table 5: Well pad and active wells variation explained among HF samples only for each dataset. Paired datasets were not subject to this analysis, as their respective HF- samples were excluded.</t>
-  </si>
-  <si>
-    <t>Metatranscriptomics microbial composition (metatranscriptome) HF+ samples</t>
-  </si>
-  <si>
     <t>WellPad_Active</t>
+  </si>
+  <si>
+    <t>Supplemental Table 5: Well pad and active wells variation explained among UOG+ samples only for each dataset. Paired datasets were not subject to this analysis, as their respective UOG- samples were excluded.</t>
+  </si>
+  <si>
+    <t>Metatranscriptomics antimicrobial resistance genes UOG+ samples</t>
+  </si>
+  <si>
+    <t>Metatranscriptomics UOG+ samples</t>
+  </si>
+  <si>
+    <t>Metatranscriptomics microbial composition (metatranscriptome) UOG+ samples</t>
+  </si>
+  <si>
+    <t>Sediment 16S rRNA gene UOG+ samples</t>
+  </si>
+  <si>
+    <t>Water 16S rRNA gene UOG+ samples</t>
   </si>
 </sst>
 </file>
@@ -399,14 +399,17 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -446,7 +449,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -466,7 +469,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -486,7 +489,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -506,7 +509,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -526,12 +529,12 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>8.3199809020000001E-2</v>
@@ -546,12 +549,12 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0.28024803949999999</v>
@@ -566,12 +569,12 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>0.18958987729999999</v>
@@ -586,12 +589,12 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>4.2472593029999998E-2</v>
@@ -606,12 +609,12 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>6.743520033E-2</v>
@@ -626,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>